<commit_message>
Added: extra stimuli with distortion
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aivan\OneDrive\Documents\University\Cognitive Psychology\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E05C1F-5380-432B-BB95-F148F5953730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA4406-19F0-46EA-9340-BB99F5C4ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,50 +96,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>video_file</t>
   </si>
   <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_ba_ba_ba_ba.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_ba_ba_da_da.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_ba_ba_va_va.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_da_da_ba_ba.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_da_da_da_da.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_da_da_va_va.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_va_va_ba_ba.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_va_va_da_da.mp4</t>
-  </si>
-  <si>
-    <t>stimuli/stimuli_va_va_va_va.mp4</t>
-  </si>
-  <si>
-    <t>congruent</t>
-  </si>
-  <si>
-    <t>non_congruent</t>
-  </si>
-  <si>
-    <t>sound</t>
-  </si>
-  <si>
     <t>ba_ba</t>
   </si>
   <si>
@@ -147,6 +108,69 @@
   </si>
   <si>
     <t>va_va</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_baba.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_dada.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_vava.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_baba.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_dada.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_vava.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_baba.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_dada.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_vava.mp4</t>
+  </si>
+  <si>
+    <t>distorted</t>
+  </si>
+  <si>
+    <t>utterance</t>
+  </si>
+  <si>
+    <t>articulation</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_baba_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_dada_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_baba_vava_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_baba_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_dada_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_dada_vava_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_baba_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_dada_dst.mp4</t>
+  </si>
+  <si>
+    <t>stimuli/stimuli_vava_vava_dst.mp4</t>
   </si>
 </sst>
 </file>
@@ -217,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,6 +249,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,128 +574,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22.625" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="20.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -685,12 +868,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -804,16 +996,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -828,7 +1019,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -842,12 +1033,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>